<commit_message>
finished gui, working on further functionality
</commit_message>
<xml_diff>
--- a/Invoice_template.xlsx
+++ b/Invoice_template.xlsx
@@ -590,7 +590,7 @@
     <row r="1" ht="30" customHeight="1" s="13">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>INVOICE #3135</t>
+          <t>INVOICE #3148</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,11 @@
           <t>Alice Bell</t>
         </is>
       </c>
-      <c r="C7" s="16" t="inlineStr"/>
+      <c r="C7" s="16" t="inlineStr">
+        <is>
+          <t>Generator Maintenace</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="30" customHeight="1" s="13">
       <c r="B8" s="0" t="inlineStr">
@@ -693,8 +697,14 @@
       </c>
     </row>
     <row r="13" ht="30" customHeight="1" s="13">
-      <c r="B13" s="0" t="inlineStr"/>
-      <c r="C13" s="8" t="inlineStr"/>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>Gen Set PM</t>
+        </is>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="14" ht="30" customHeight="1" s="13">
       <c r="B14" s="4" t="inlineStr">

</xml_diff>